<commit_message>
modified:   cmv.docx 	new file:   collage.png 	new file:   data/disease_incidence.csv 	new file:   data/refseqs/edited/combine.py 	new file:   data/refseqs/edited/sdt.fasta 	deleted:    data/seq.zip 	new file:   data/seqs/edited/combine.py 	new file:   data/seqs/edited/sdt.fasta 	new file:   data/srilanka/edited/combine.py 	new file:   data/srilanka/edited/sdt.fasta 	new file:   diseaseinc.png 	modified:   ext/Disease incidence.xlsx 	deleted:    ext/pics/1.jpg 	deleted:    ext/pics/4.jpg 	new file:   ext/pics/4.png 	deleted:    ext/pics/5.jpg 	new file:   ext/pics/5.png 	new file:   ext/pics/6.png 	new file:   ext/pics/7.png 	new file:   ext/pics/8.png 	new file:   ext/pics/9.png 	new file:   ext/pics/pics.pptx 	new file:   ext/~$ssava draft.docx 	modified:   plots.ipynb 	new file:   srilanka_mat.bmp 	deleted:    table.docx 	new file:   ~$cmv.docx 	new file:   ~WRL3631.tmp
</commit_message>
<xml_diff>
--- a/ext/Disease incidence.xlsx
+++ b/ext/Disease incidence.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anoban\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cmv\ext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F694F1-DDF7-4A2F-9EA6-963A4FBEBD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AC19F9-22BC-4744-ACBC-AC08007A2D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
+    <sheet name="DI" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>L1</t>
   </si>
@@ -57,6 +58,24 @@
   </si>
   <si>
     <t xml:space="preserve">    &lt;------   % of Disease incidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padavisripura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muthur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nilaveli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuchchaveli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kinniya </t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -136,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +168,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,4 +1702,145 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3C5290-8CB5-4B4D-85D3-4B506D72D30A}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>58.5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>51.3</v>
+      </c>
+      <c r="D2" s="7">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7">
+        <v>35.5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>35.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>62.4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45.5</v>
+      </c>
+      <c r="D3" s="7">
+        <v>50.55</v>
+      </c>
+      <c r="E3" s="7">
+        <v>38.75</v>
+      </c>
+      <c r="F3" s="7">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>52.8</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42</v>
+      </c>
+      <c r="D4" s="7">
+        <v>55.54</v>
+      </c>
+      <c r="E4" s="7">
+        <v>42.55</v>
+      </c>
+      <c r="F4" s="7">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>48.5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>39.75</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43.5</v>
+      </c>
+      <c r="E5" s="7">
+        <v>45.75</v>
+      </c>
+      <c r="F5" s="7">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>54</v>
+      </c>
+      <c r="C6" s="7">
+        <v>41.25</v>
+      </c>
+      <c r="D6" s="7">
+        <v>48</v>
+      </c>
+      <c r="E6" s="7">
+        <v>46.85</v>
+      </c>
+      <c r="F6" s="7">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   BLAST-Scraping.ipynb 	modified:   CMVS.xlsx 	new file:   alignment-samples.jpg 	new file:   alignment-samples.png 	new file:   all_mat.bmp modified:   cmv.docx 	new file:   collage-.png 	new file:   combined.png 	new file:   combined_matrix.csv 	new file:   data/BLAST/metainfo.csv 	new file:   data/allaligned.fasta 	new file:   data/allseqs.fasta 	deleted:    data/disease_incidence.csv 	renamed:    data/seqs/edited/matrix_mat.txt -> data/seqs/edited/matrix_mat.csv 	modified:   data/seqs/edited/sdt.fasta 	new file:   data/seqs/edited/stdaligned.fasta 	new file:   data/supplement.xlsx 	modified:   ext/Disease incidence.xlsx 	modified:   samples.png 	new file:   tree.png 	new file:   ~$cmv.docx
</commit_message>
<xml_diff>
--- a/ext/Disease incidence.xlsx
+++ b/ext/Disease incidence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cmv\ext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AC19F9-22BC-4744-ACBC-AC08007A2D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DAFBC3-8B8E-4621-B1A0-CAAA5597CEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>L1</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Site</t>
+  </si>
+  <si>
+    <t>AVE</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1477,7 +1480,7 @@
   <dimension ref="B4:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F9"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1706,18 +1709,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3C5290-8CB5-4B4D-85D3-4B506D72D30A}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1840,6 +1845,37 @@
         <v>44</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(B$2:B$6)</f>
+        <v>55.239999999999995</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="0">AVERAGE(C$2:C$6)</f>
+        <v>43.96</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>50.718000000000004</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>41.88</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>39.411999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>MIN(B2:F6)</f>
+        <v>35.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>